<commit_message>
added milestones in MPP
</commit_message>
<xml_diff>
--- a/MGMT/PLAN/WBS/WORK IN PROGRESS/RAM_MWBS.xlsx
+++ b/MGMT/PLAN/WBS/WORK IN PROGRESS/RAM_MWBS.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmb/learning/MTECH/2nd year PROJECT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmb/learning/MTECH/SE25PT7SERIS/MGMT/PLAN/WBS/WORK IN PROGRESS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA850A15-3A3D-5942-BA1E-A608C925ED91}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8F710E-8347-9D4C-BCD1-5FDCB89633FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="460" windowWidth="25600" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="2" r:id="rId1"/>
+    <sheet name="Milestones" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="171">
   <si>
     <t>Task</t>
   </si>
@@ -323,6 +324,216 @@
   </si>
   <si>
     <t>William</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>Project Milestones</t>
+  </si>
+  <si>
+    <t>Approx. Date</t>
+  </si>
+  <si>
+    <t>Issue Prototype Study Report</t>
+  </si>
+  <si>
+    <t>Issue Risk Tracker</t>
+  </si>
+  <si>
+    <t>Issue User Interface Specification Doc</t>
+  </si>
+  <si>
+    <t>Issue High Level Design Doc</t>
+  </si>
+  <si>
+    <t>Issue Quality Plan Doc</t>
+  </si>
+  <si>
+    <t>Implement Prototype</t>
+  </si>
+  <si>
+    <t>Issue Work Breakdown Structure</t>
+  </si>
+  <si>
+    <t>Issue Use Case Modelling Survey Report</t>
+  </si>
+  <si>
+    <t>Issue Project Plan Doc</t>
+  </si>
+  <si>
+    <t>Issue User Requirement Specification Doc</t>
+  </si>
+  <si>
+    <t>Increment 0</t>
+  </si>
+  <si>
+    <t>Increment 1</t>
+  </si>
+  <si>
+    <t>Setup Cloud Environment</t>
+  </si>
+  <si>
+    <t>Issue Use Case Modelling Survey Report(Analysis)</t>
+  </si>
+  <si>
+    <t>Issue Design Report</t>
+  </si>
+  <si>
+    <t>Complete Source Control Plan and Setup</t>
+  </si>
+  <si>
+    <t>Complete Coding</t>
+  </si>
+  <si>
+    <t>Issue System Test Plan</t>
+  </si>
+  <si>
+    <t>Complete System Testing</t>
+  </si>
+  <si>
+    <t>Complete Integration Test</t>
+  </si>
+  <si>
+    <t>Issue SIT Document</t>
+  </si>
+  <si>
+    <t>Issue User Acceptance Test Plan</t>
+  </si>
+  <si>
+    <t>Issue End User Traning Manual and User Guide</t>
+  </si>
+  <si>
+    <t>Complete User Acceptance Testing</t>
+  </si>
+  <si>
+    <t>Issue User Acceptance Test Document</t>
+  </si>
+  <si>
+    <t>Increment 2</t>
+  </si>
+  <si>
+    <t>Project Hand-over</t>
+  </si>
+  <si>
+    <t>Commence User Traning</t>
+  </si>
+  <si>
+    <t>Complete AWS setup and manual</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>2.10</t>
+  </si>
+  <si>
+    <t>2.11</t>
+  </si>
+  <si>
+    <t>2.12</t>
+  </si>
+  <si>
+    <t>2.13</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>3.11</t>
+  </si>
+  <si>
+    <t>3.12</t>
+  </si>
+  <si>
+    <t>3.13</t>
+  </si>
+  <si>
+    <t>3.14</t>
+  </si>
+  <si>
+    <t>3.15</t>
+  </si>
+  <si>
+    <t>3.16</t>
   </si>
 </sst>
 </file>
@@ -373,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -386,10 +597,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -708,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BA2D23-3C83-1247-BC0F-C7121E9E977D}">
   <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -719,29 +947,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>100</v>
       </c>
     </row>
@@ -785,15 +1013,15 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9"/>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
@@ -922,80 +1150,86 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41">
+    <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
         <v>6</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>7</v>
       </c>
@@ -1003,7 +1237,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
         <v>48</v>
       </c>
@@ -1369,4 +1603,488 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D043F0-DDA8-414F-B24E-F1B01A83E36A}">
+  <dimension ref="A1:C43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection sqref="A1:C43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5" style="11" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" style="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="9">
+        <v>43165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="9">
+        <v>43187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="9">
+        <v>43205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="9">
+        <v>43174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="9">
+        <v>43202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="9">
+        <v>43205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="9">
+        <v>43207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="9">
+        <v>43204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="9">
+        <v>43204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="9">
+        <v>43205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="9">
+        <v>43222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="9">
+        <v>43226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="9">
+        <v>43240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="9">
+        <v>43221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="9">
+        <v>43296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="9">
+        <v>43240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="9">
+        <v>43303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="9">
+        <v>43310</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="9">
+        <v>43317</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="9">
+        <v>43317</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="9">
+        <v>43324</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="9">
+        <v>43331</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="9">
+        <v>43306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="9">
+        <v>43345</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="9">
+        <v>43352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="9">
+        <v>43359</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="9">
+        <v>43345</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="9">
+        <v>43422</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="9">
+        <v>43427</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="9">
+        <v>43429</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="9">
+        <v>43436</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="9">
+        <v>43443</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="9">
+        <v>43443</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38" s="9">
+        <v>43450</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" s="9">
+        <v>43443</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" s="9">
+        <v>43450</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="9">
+        <v>43457</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C42" s="9">
+        <v>43457</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="9">
+        <v>43465</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A27:C27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>